<commit_message>
Fixup sample spreadsheet to match the paper
</commit_message>
<xml_diff>
--- a/static/Sample.xlsx
+++ b/static/Sample.xlsx
@@ -504,17 +504,17 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="9"/>
   </cols>
   <sheetData>
@@ -993,7 +993,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="19" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C9" s="20" t="n">
         <v>3</v>
@@ -1109,7 +1109,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="23" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C11" s="11" t="n">
         <v>10</v>

</xml_diff>